<commit_message>
Coding Data Functionality update
</commit_message>
<xml_diff>
--- a/SMLToolbox/RecodingDataSets/RecodingImages/codedimagedata.xlsx
+++ b/SMLToolbox/RecodingDataSets/RecodingImages/codedimagedata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmgco\Documents\GitHub\SML\SMLToolBox\RecodingDataSets\RecodingImages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0557127D-2425-4842-8236-6E145E6D0A43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C689DEC-8F64-4C46-A0AF-C1AA4AF89072}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="9420" xr2:uid="{667EA247-433E-4711-A7AD-91D6EF421685}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="9615" xr2:uid="{B3961FDA-0045-474A-9EF1-954EEC464C91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,56 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f6</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>f8</t>
+  </si>
+  <si>
+    <t>f9</t>
+  </si>
+  <si>
+    <t>f10</t>
+  </si>
+  <si>
+    <t>f11</t>
+  </si>
+  <si>
+    <t>f12</t>
+  </si>
+  <si>
+    <t>f13</t>
+  </si>
+  <si>
+    <t>f14</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,201 +420,248 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDF1B43-9662-4F4C-9C0B-7AC88D0C7C04}">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A61B7D2-27C0-47F7-BEE3-029A1F802F52}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O4"/>
+      <selection sqref="A1:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0.98538950348028997</v>
-      </c>
-      <c r="B1">
-        <v>0.10563894528931224</v>
-      </c>
-      <c r="C1">
-        <v>0.10046774502926965</v>
-      </c>
-      <c r="D1">
-        <v>3.801752165048896E-2</v>
-      </c>
-      <c r="E1">
-        <v>2.0799912435065456E-2</v>
-      </c>
-      <c r="F1">
-        <v>3.9949013933146503E-2</v>
-      </c>
-      <c r="G1">
-        <v>5.0586475738047365E-2</v>
-      </c>
-      <c r="H1">
-        <v>2.8155693205916363E-2</v>
-      </c>
-      <c r="I1">
-        <v>3.9317695539450876E-3</v>
-      </c>
-      <c r="J1">
-        <v>1.5275764776695608E-2</v>
-      </c>
-      <c r="K1">
-        <v>7.7297707465816372E-3</v>
-      </c>
-      <c r="L1">
-        <v>1.8299506708648043E-2</v>
-      </c>
-      <c r="M1">
-        <v>1.4162830989866801E-2</v>
-      </c>
-      <c r="N1">
-        <v>8.3145467772051136E-3</v>
-      </c>
-      <c r="O1">
-        <v>3.9241169208037319E-3</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.99189230520297633</v>
+        <v>0.10563894528931221</v>
       </c>
       <c r="B2">
-        <v>5.4966196053412478E-2</v>
+        <v>0.10046774502926963</v>
       </c>
       <c r="C2">
-        <v>4.4563140784203599E-2</v>
+        <v>3.8017521650488953E-2</v>
       </c>
       <c r="D2">
-        <v>5.6143851780417191E-2</v>
+        <v>2.0799912435065453E-2</v>
       </c>
       <c r="E2">
-        <v>2.3484171583938094E-2</v>
+        <v>3.9949013933146496E-2</v>
       </c>
       <c r="F2">
-        <v>1.2127697361843826E-2</v>
+        <v>5.0586475738047351E-2</v>
       </c>
       <c r="G2">
-        <v>1.4145319718717114E-2</v>
+        <v>2.8155693205916356E-2</v>
       </c>
       <c r="H2">
-        <v>2.4317825849495014E-2</v>
+        <v>3.9317695539450867E-3</v>
       </c>
       <c r="I2">
-        <v>3.0546846457921693E-2</v>
+        <v>1.5275764776695604E-2</v>
       </c>
       <c r="J2">
-        <v>2.3729714935879855E-2</v>
+        <v>7.7297707465816354E-3</v>
       </c>
       <c r="K2">
-        <v>3.2379939049302746E-2</v>
+        <v>1.829950670864804E-2</v>
       </c>
       <c r="L2">
-        <v>2.3976529530875659E-2</v>
+        <v>1.4162830989866797E-2</v>
       </c>
       <c r="M2">
-        <v>2.3721064964841717E-2</v>
+        <v>8.3145467772051118E-3</v>
       </c>
       <c r="N2">
-        <v>3.2799314988443781E-2</v>
+        <v>3.9241169208037311E-3</v>
       </c>
       <c r="O2">
-        <v>4.1740925619264242E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.97113322472150188</v>
+        <v>5.4966196053412464E-2</v>
       </c>
       <c r="B3">
-        <v>0.21044496538405799</v>
+        <v>4.4563140784203592E-2</v>
       </c>
       <c r="C3">
-        <v>2.025603121446682E-2</v>
+        <v>5.6143851780417177E-2</v>
       </c>
       <c r="D3">
-        <v>4.3067639798329165E-2</v>
+        <v>2.3484171583938087E-2</v>
       </c>
       <c r="E3">
-        <v>3.6204669271263645E-2</v>
+        <v>1.2127697361843822E-2</v>
       </c>
       <c r="F3">
-        <v>5.1327600406608213E-2</v>
+        <v>1.414531971871711E-2</v>
       </c>
       <c r="G3">
-        <v>1.4147930756331369E-2</v>
+        <v>2.4317825849495007E-2</v>
       </c>
       <c r="H3">
-        <v>4.8477617045863626E-2</v>
+        <v>3.0546846457921686E-2</v>
       </c>
       <c r="I3">
-        <v>4.1229840201382789E-2</v>
+        <v>2.3729714935879848E-2</v>
       </c>
       <c r="J3">
-        <v>1.9875578529320103E-2</v>
+        <v>3.2379939049302739E-2</v>
       </c>
       <c r="K3">
-        <v>2.4729482812973037E-2</v>
+        <v>2.3976529530875652E-2</v>
       </c>
       <c r="L3">
-        <v>1.9170943265950497E-2</v>
+        <v>2.372106496484171E-2</v>
       </c>
       <c r="M3">
-        <v>1.6885343449921944E-2</v>
+        <v>3.2799314988443774E-2</v>
       </c>
       <c r="N3">
-        <v>1.7668996577541576E-2</v>
+        <v>4.1740925619264235E-2</v>
       </c>
       <c r="O3">
-        <v>1.3460499775156962E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.97228070446308368</v>
+        <v>0.21044496538405794</v>
       </c>
       <c r="B4">
+        <v>2.0256031214466817E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.3067639798329158E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.6204669271263638E-2</v>
+      </c>
+      <c r="E4">
+        <v>5.13276004066082E-2</v>
+      </c>
+      <c r="F4">
+        <v>1.4147930756331365E-2</v>
+      </c>
+      <c r="G4">
+        <v>4.8477617045863612E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.1229840201382782E-2</v>
+      </c>
+      <c r="I4">
+        <v>1.98755785293201E-2</v>
+      </c>
+      <c r="J4">
+        <v>2.472948281297303E-2</v>
+      </c>
+      <c r="K4">
+        <v>1.9170943265950494E-2</v>
+      </c>
+      <c r="L4">
+        <v>1.6885343449921941E-2</v>
+      </c>
+      <c r="M4">
+        <v>1.7668996577541573E-2</v>
+      </c>
+      <c r="N4">
+        <v>1.3460499775156958E-2</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3.2048952257576334E-2</v>
       </c>
-      <c r="C4">
+      <c r="B5">
         <v>0.14092777348728899</v>
       </c>
-      <c r="D4">
+      <c r="C5">
         <v>6.9321869291812957E-2</v>
       </c>
-      <c r="E4">
+      <c r="D5">
         <v>7.9916306112718799E-2</v>
       </c>
-      <c r="F4">
+      <c r="E5">
         <v>4.6430101614712393E-2</v>
       </c>
-      <c r="G4">
+      <c r="F5">
         <v>6.8769018995263845E-2</v>
       </c>
-      <c r="H4">
+      <c r="G5">
         <v>3.3817452989021259E-2</v>
       </c>
-      <c r="I4">
+      <c r="H5">
         <v>5.5505273539062476E-2</v>
       </c>
-      <c r="J4">
+      <c r="I5">
         <v>5.8870966777792418E-2</v>
       </c>
-      <c r="K4">
+      <c r="J5">
         <v>4.4833408833361649E-2</v>
       </c>
-      <c r="L4">
+      <c r="K5">
         <v>4.2444682292264099E-2</v>
       </c>
-      <c r="M4">
+      <c r="L5">
         <v>4.6985400130180814E-2</v>
       </c>
-      <c r="N4">
+      <c r="M5">
         <v>3.647005230650012E-2</v>
       </c>
-      <c r="O4">
+      <c r="N5">
         <v>2.5804356293747235E-2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>